<commit_message>
ChkPoint: clean up scripts a4.6_all_data_preparation.py a5.2_pd_model_data_prep.py
</commit_message>
<xml_diff>
--- a/data/1.1_lc_data_dictionary.xlsx
+++ b/data/1.1_lc_data_dictionary.xlsx
@@ -5,23 +5,23 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\al_files\PycharmProjects\Python\CreditRiskModelingPython2020\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\al_files\PycharmProjects\Python\CreditRiskModelingPython2022\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D81D6D7-61AB-4353-AC02-9FDBD2ACE8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23624496-F294-4B8B-905C-4379577E57DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29040" yWindow="615" windowWidth="25020" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
-    <sheet name="LoanStats (2)" sheetId="8" r:id="rId2"/>
+    <sheet name="LoanStats (2)" sheetId="9" r:id="rId2"/>
     <sheet name="browseNotes" sheetId="6" r:id="rId3"/>
     <sheet name="RejectStats" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">browseNotes!$A$1:$B$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$M$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'LoanStats (2)'!$A$1:$F$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'LoanStats (2)'!$A$1:$M$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="320">
   <si>
     <t>id</t>
   </si>
@@ -933,18 +933,6 @@
   </si>
   <si>
     <t>Debt to Income Ratio. A ratio calculated using the borrower’s total monthly debt payments on the total debt obligations, excluding mortgage and the requested LC loan, divided by the borrower’s self-reported monthly income.</t>
-  </si>
-  <si>
-    <t>PD_Variable</t>
-  </si>
-  <si>
-    <t>Is_Discrete</t>
-  </si>
-  <si>
-    <t>Is_Preprocessed</t>
-  </si>
-  <si>
-    <t>New_Name</t>
   </si>
   <si>
     <t>emp_length_int</t>
@@ -1198,7 +1186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1387,12 +1375,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1646,7 +1628,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1657,7 +1639,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1666,7 +1647,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1676,6 +1656,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2076,7 +2057,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,79 +2074,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="J1" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>A2&amp;":category i"</f>
-        <v>addr_state:category i</v>
-      </c>
-      <c r="J2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>260</v>
-      </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2175,46 +2149,62 @@
       </c>
       <c r="G3" t="str">
         <f>A3&amp;":category i"</f>
+        <v>addr_state:category i</v>
+      </c>
+      <c r="J3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <f>A5&amp;":category i"</f>
         <v>annual_inc:category i</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2222,254 +2212,239 @@
     </row>
     <row r="7" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>323</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>319</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>300</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>301</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>297</v>
+      </c>
+      <c r="H15" s="15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>262</v>
+        <v>168</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>261</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" ref="G19:G20" si="0">A19&amp;":category i"</f>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="str">
+        <f>A21&amp;":category i"</f>
         <v>grade:category i</v>
       </c>
-      <c r="J19" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="J21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>home_ownership:category i</v>
-      </c>
-      <c r="J20" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2485,206 +2460,208 @@
       </c>
       <c r="G22" t="str">
         <f>A22&amp;":category i"</f>
-        <v>initial_list_status:category i</v>
+        <v>home_ownership:category i</v>
       </c>
       <c r="J22" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>263</v>
+        <v>63</v>
       </c>
       <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>323</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>7</v>
+        <v>279</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="str">
+        <f>A25&amp;":category i"</f>
+        <v>initial_list_status:category i</v>
+      </c>
+      <c r="J25" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>289</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>14</v>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>291</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>249</v>
+        <v>292</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="G27" t="s">
-        <v>305</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>319</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>301</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="str">
-        <f>A34&amp;":category i"</f>
-        <v>loan_status:category i</v>
-      </c>
-      <c r="J34" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C35">
         <v>0</v>
       </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2692,268 +2669,222 @@
     </row>
     <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>45</v>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="str">
+        <f>A39&amp;":category i"</f>
+        <v>loan_status:category i</v>
+      </c>
+      <c r="J39" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>30</v>
+        <v>285</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>76</v>
+        <v>286</v>
       </c>
       <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>323</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="J40" t="s">
-        <v>314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>31</v>
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="J44" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>238</v>
+        <v>276</v>
       </c>
       <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45" t="str">
-        <f>A45&amp;":category i"</f>
-        <v>purpose:category i</v>
-      </c>
-      <c r="J45" t="s">
-        <v>311</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>226</v>
+        <v>30</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>224</v>
+        <v>76</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>319</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>32</v>
+        <v>267</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>79</v>
+        <v>268</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>33</v>
+        <v>271</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>80</v>
+        <v>272</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>9</v>
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>81</v>
+        <v>274</v>
       </c>
       <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" t="str">
-        <f>A50&amp;":category i"</f>
-        <v>sub_grade:category i</v>
-      </c>
-      <c r="J50" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>82</v>
+        <v>270</v>
       </c>
       <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="G51" t="s">
-        <v>306</v>
-      </c>
-      <c r="J51" t="s">
-        <v>303</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>20</v>
+        <v>281</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>83</v>
+        <v>282</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>34</v>
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>284</v>
       </c>
       <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="J53" t="s">
-        <v>314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2961,92 +2892,101 @@
     </row>
     <row r="55" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>96</v>
+        <v>241</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>42</v>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>97</v>
+        <v>238</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58" t="str">
+        <f>A58&amp;":category i"</f>
+        <v>purpose:category i</v>
+      </c>
+      <c r="J58" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
-        <v>309</v>
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>310</v>
+        <v>224</v>
       </c>
       <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60" t="str">
-        <f>A60&amp;":category i"</f>
-        <v>verification_status:category i</v>
-      </c>
-      <c r="J60" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>258</v>
+        <v>32</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>259</v>
+        <v>79</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3054,43 +2994,71 @@
     </row>
     <row r="62" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>248</v>
+        <v>33</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>247</v>
+        <v>80</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>267</v>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>268</v>
+        <v>81</v>
       </c>
       <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>269</v>
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="str">
+        <f>A63&amp;":category i"</f>
+        <v>sub_grade:category i</v>
+      </c>
+      <c r="J63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>270</v>
+        <v>82</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>302</v>
+      </c>
+      <c r="J64" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>271</v>
+        <v>20</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>272</v>
+        <v>83</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -3098,10 +3066,10 @@
     </row>
     <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>273</v>
+        <v>129</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>274</v>
+        <v>157</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3109,32 +3077,41 @@
     </row>
     <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>275</v>
+        <v>114</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>276</v>
+        <v>156</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="J68" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -3142,10 +3119,10 @@
     </row>
     <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -3153,21 +3130,21 @@
     </row>
     <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>283</v>
+        <v>38</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>284</v>
+        <v>93</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>285</v>
+        <v>39</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>286</v>
+        <v>94</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -3175,105 +3152,112 @@
     </row>
     <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>287</v>
+        <v>41</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>218</v>
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="J74" t="s">
-        <v>312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>289</v>
+        <v>40</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>290</v>
+        <v>97</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>295</v>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
+        <v>218</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>294</v>
+        <v>159</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="J76" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>291</v>
+        <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>292</v>
+        <v>87</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>50</v>
+        <v>306</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78" t="str">
+        <f>A78&amp;":category i"</f>
+        <v>verification_status:category i</v>
       </c>
       <c r="J78" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>157</v>
+        <v>259</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>114</v>
+        <v>248</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3292,8 +3276,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B102">
-    <sortCondition ref="A2:A102"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J80">
+    <sortCondition ref="A1:A80"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3306,53 +3290,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058B74A3-4964-4012-B180-CF5AED18A55B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C429C9E2-C5DF-4606-BCF8-C616C54A829D}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="42.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="E1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -3362,9 +3361,25 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>A2&amp;":category i"</f>
+        <v>addr_state:category i</v>
+      </c>
+      <c r="J2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3373,30 +3388,52 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>A3&amp;":category i"</f>
+        <v>annual_inc:category i</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>266</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>254</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>227</v>
       </c>
@@ -3407,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>107</v>
       </c>
@@ -3418,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -3426,10 +3463,19 @@
         <v>55</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>319</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -3440,41 +3486,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>296</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>257</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>300</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3489,14 +3550,17 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>301</v>
-      </c>
       <c r="G13" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>167</v>
       </c>
@@ -3507,42 +3571,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="10">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="10">
-        <v>0</v>
-      </c>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -3553,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>8</v>
       </c>
@@ -3563,8 +3633,24 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ref="G19:G20" si="0">A19&amp;":category i"</f>
+        <v>grade:category i</v>
+      </c>
+      <c r="J19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3574,31 +3660,63 @@
       <c r="C20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>home_ownership:category i</v>
+      </c>
+      <c r="J20" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="str">
+        <f>A22&amp;":category i"</f>
+        <v>initial_list_status:category i</v>
+      </c>
+      <c r="J22" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3607,8 +3725,17 @@
       <c r="C23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>319</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3619,18 +3746,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3641,18 +3768,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>249</v>
       </c>
       <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>301</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
@@ -3663,31 +3802,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="10">
-        <v>0</v>
-      </c>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="10">
-        <v>0</v>
-      </c>
-      <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -3698,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
@@ -3709,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3720,8 +3865,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -3730,19 +3875,35 @@
       <c r="C34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="str">
+        <f>A34&amp;":category i"</f>
+        <v>loan_status:category i</v>
+      </c>
+      <c r="J34" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
@@ -3753,18 +3914,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>29</v>
       </c>
@@ -3775,7 +3936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
@@ -3786,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>30</v>
       </c>
@@ -3794,10 +3955,19 @@
         <v>76</v>
       </c>
       <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>319</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -3808,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -3819,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>130</v>
       </c>
@@ -3830,18 +4000,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>19</v>
       </c>
@@ -3851,8 +4030,24 @@
       <c r="C45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="str">
+        <f>A45&amp;":category i"</f>
+        <v>purpose:category i</v>
+      </c>
+      <c r="J45" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -3863,18 +4058,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>224</v>
       </c>
       <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>32</v>
       </c>
@@ -3885,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>33</v>
       </c>
@@ -3896,19 +4091,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" t="str">
+        <f>A50&amp;":category i"</f>
+        <v>sub_grade:category i</v>
+      </c>
+      <c r="J50" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3917,8 +4128,20 @@
       <c r="C51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>302</v>
+      </c>
+      <c r="J51" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -3929,18 +4152,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="J53" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>38</v>
       </c>
@@ -3951,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>39</v>
       </c>
@@ -3962,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>41</v>
       </c>
@@ -3973,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>42</v>
       </c>
@@ -3984,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -3995,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
@@ -4006,235 +4238,279 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="str">
+        <f>A60&amp;":category i"</f>
+        <v>verification_status:category i</v>
+      </c>
+      <c r="J60" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="J74" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="J78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F79" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
+  <pageSetup scale="64" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4290,7 +4566,7 @@
       <c r="A5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4991,10 +5267,10 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" s="7" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5149,10 +5425,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>